<commit_message>
Påbörjar utvecklings fas fasen nu
</commit_message>
<xml_diff>
--- a/Pilot test data.xlsx
+++ b/Pilot test data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusliljenberg/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusliljenberg/Documents/ExJobb/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{13033299-4804-1445-B7A5-D1C50866F8B9}"/>
+    <workbookView minimized="1" xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{13033299-4804-1445-B7A5-D1C50866F8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>BBC-ZH</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>BBC-Eng</t>
+  </si>
+  <si>
+    <t>60x</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>1.20x</t>
+  </si>
+  <si>
+    <t>QQ-eng</t>
   </si>
 </sst>
 </file>
@@ -402,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2158BDB-21FE-6548-A4C1-C3226344AC92}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E15" sqref="E15:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,6 +628,209 @@
         <v>5</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>45</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>